<commit_message>
Update & Add Part of UI
</commit_message>
<xml_diff>
--- a/TheGoat/Content/Data/Raw/PlayerAttack.xlsx
+++ b/TheGoat/Content/Data/Raw/PlayerAttack.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Colythme\Project\COMP4451-Code\TheGoat\Content\Data\Raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Colythme\Project\The-Goat\TheGoat\Content\Data\Raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECD45D5-1FB9-4B7C-B164-1F2E2168E0DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E238041D-1A54-4CD5-8813-0D3D7A82D87F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Damage</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -57,6 +57,14 @@
   </si>
   <si>
     <t>HeavyAttackCombo02</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rage Increase</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Impact</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -408,20 +416,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.625" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="1"/>
+    <col min="3" max="3" width="9" style="1"/>
+    <col min="4" max="4" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -429,8 +439,14 @@
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -440,8 +456,14 @@
       <c r="C2" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -451,8 +473,14 @@
       <c r="C3" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -462,8 +490,14 @@
       <c r="C4" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -473,8 +507,14 @@
       <c r="C5" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -484,8 +524,14 @@
       <c r="C6" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -495,8 +541,14 @@
       <c r="C7" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" s="2">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -505,6 +557,12 @@
       </c>
       <c r="C8" s="2">
         <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>